<commit_message>
fix some bugs after testing
</commit_message>
<xml_diff>
--- a/start_table/sample.xlsx
+++ b/start_table/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergejbostan/Desktop/testsProjects/avito_parser/ads_count/start_table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergejbostan/Desktop/testsProjects/avito_parser/ads_count/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFFE1FD-DA94-1449-BADA-1B2AB36D75F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8818BA-5372-7946-AF00-78AD59544020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{84CBCFBE-DB81-EF41-AB67-AC517E5EE53F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>пластиковые окна</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Краснодарский край, Славянск-на-Кубани</t>
+  </si>
+  <si>
+    <t>Краснодарский край, Туапсе</t>
   </si>
   <si>
     <t>Краснодарский край, Лабинск</t>
@@ -523,12 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -563,6 +560,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -881,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAE9602-8374-0E48-ACA6-840B1149C90A}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,119 +898,119 @@
   <sheetData>
     <row r="1" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="19"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="22"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="24"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="22"/>
     </row>
     <row r="6" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -1140,7 +1143,9 @@
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1157,7 +1162,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
@@ -1175,7 +1180,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="6"/>
@@ -1193,7 +1198,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="6"/>
@@ -1211,7 +1216,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
@@ -1229,7 +1234,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="6"/>
@@ -1247,7 +1252,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="6"/>
@@ -1265,7 +1270,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="6"/>
@@ -1283,7 +1288,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="6"/>
@@ -1301,7 +1306,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="6"/>
@@ -1319,7 +1324,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="6"/>
@@ -1337,7 +1342,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="6"/>
@@ -1355,7 +1360,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="6"/>
@@ -1373,7 +1378,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="6"/>
@@ -1391,7 +1396,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="6"/>
@@ -1409,7 +1414,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="6"/>
@@ -1427,7 +1432,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="6"/>
@@ -1445,7 +1450,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="6"/>
@@ -1463,7 +1468,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="6"/>
@@ -1481,7 +1486,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="6"/>
@@ -1499,7 +1504,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="6"/>
@@ -1517,7 +1522,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="6"/>
@@ -1535,7 +1540,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="6"/>
@@ -1553,7 +1558,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="6"/>
@@ -1571,7 +1576,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="6"/>
@@ -1589,7 +1594,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="6"/>
@@ -1607,7 +1612,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="6"/>
@@ -1625,7 +1630,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="6"/>
@@ -1643,7 +1648,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="6"/>
@@ -1661,7 +1666,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="6"/>
@@ -1679,7 +1684,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="6"/>
@@ -1697,7 +1702,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="6"/>
@@ -1715,7 +1720,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="6"/>
@@ -1733,7 +1738,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="6"/>
@@ -1751,7 +1756,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="6"/>
@@ -1769,7 +1774,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="6"/>
@@ -1787,7 +1792,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="6"/>
@@ -1805,7 +1810,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="6"/>
@@ -1823,7 +1828,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="6"/>
@@ -1841,7 +1846,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="6"/>
@@ -1859,7 +1864,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="6"/>
@@ -1877,7 +1882,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="6"/>
@@ -1895,7 +1900,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="6"/>
@@ -1913,7 +1918,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="6"/>
@@ -1931,7 +1936,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="6"/>
@@ -1949,7 +1954,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="6"/>
@@ -1967,7 +1972,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="6"/>
@@ -1985,7 +1990,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="6"/>
@@ -2003,7 +2008,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="6"/>
@@ -2021,7 +2026,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="6"/>
@@ -2039,7 +2044,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="6"/>
@@ -2057,7 +2062,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="6"/>
@@ -2075,7 +2080,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="6"/>
@@ -2093,7 +2098,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="6"/>
@@ -2111,7 +2116,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="6"/>
@@ -2129,7 +2134,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="6"/>
@@ -2147,7 +2152,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="6"/>
@@ -2165,7 +2170,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="6"/>
@@ -2183,7 +2188,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="6"/>
@@ -2201,7 +2206,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="6"/>
@@ -2219,7 +2224,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="6"/>
@@ -2237,7 +2242,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="6"/>
@@ -2255,7 +2260,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="6"/>
@@ -2273,7 +2278,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="6"/>
@@ -2291,7 +2296,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="6"/>
@@ -2309,7 +2314,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="6"/>
@@ -2327,7 +2332,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="6"/>
@@ -2345,7 +2350,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="6"/>
@@ -2363,7 +2368,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="6"/>
@@ -2381,7 +2386,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="6"/>
@@ -2399,7 +2404,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="6"/>
@@ -2417,7 +2422,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="6"/>
@@ -2435,7 +2440,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="6"/>
@@ -2453,7 +2458,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="6"/>
@@ -2471,7 +2476,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="6"/>
@@ -2489,7 +2494,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="6"/>
@@ -2507,7 +2512,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="6"/>
@@ -2525,7 +2530,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="6"/>
@@ -2543,7 +2548,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="6"/>
@@ -2561,7 +2566,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="6"/>
@@ -2579,7 +2584,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="6"/>
@@ -2597,7 +2602,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="6"/>
@@ -2615,7 +2620,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="6"/>
@@ -2633,7 +2638,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="6"/>
@@ -2651,7 +2656,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="6"/>
@@ -2669,7 +2674,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="6"/>
@@ -2687,7 +2692,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="6"/>
@@ -2705,7 +2710,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="6"/>
@@ -2723,7 +2728,7 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="6"/>
@@ -2741,7 +2746,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="1"/>
@@ -2759,7 +2764,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="1"/>
@@ -2777,7 +2782,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="1"/>
@@ -2795,7 +2800,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="1"/>
@@ -2813,7 +2818,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="1"/>

</xml_diff>